<commit_message>
removed unnecessary parts for preprocessing
</commit_message>
<xml_diff>
--- a/Project Plan and Resources/ProjectMonitor.xlsx
+++ b/Project Plan and Resources/ProjectMonitor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" tabRatio="869" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" tabRatio="869" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="130">
   <si>
     <t>Resources</t>
   </si>
@@ -820,6 +820,10 @@
 !!! How to push exisiting project in Eclipse to an existing repository in bitbucket?
 * Don’t intend to use maven as of now, as git can do most of what maven does. BUT NEED TO EXPLORE MORE ON THIS
 Project is now Maven</t>
+  </si>
+  <si>
+    <t>8/17/2015 2:38 PM
+!!! Need to look into friendsoffriends.java. Seems useful for DTC</t>
   </si>
 </sst>
 </file>
@@ -2314,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2683,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3102,81 +3106,86 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="19">
-        <v>28</v>
-      </c>
-      <c r="B33" s="21">
-        <v>10</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>75</v>
+    <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E33" s="34" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
+        <v>28</v>
+      </c>
+      <c r="B34" s="21">
+        <v>10</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="19">
         <v>29</v>
       </c>
-      <c r="B34" s="21">
+      <c r="B35" s="21">
         <v>11</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B35" s="23"/>
-      <c r="C35" s="23" t="s">
+    <row r="36" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B36" s="23"/>
+      <c r="C36" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="25" t="s">
+      <c r="D36" s="23"/>
+      <c r="E36" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="23"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
-        <v>30</v>
-      </c>
-      <c r="B36" s="21">
-        <v>12</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>77</v>
-      </c>
+      <c r="F36" s="23"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
-        <v>31</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+        <v>30</v>
+      </c>
+      <c r="B37" s="21">
+        <v>12</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
-        <v>32</v>
-      </c>
-      <c r="B38" s="21">
-        <v>13</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>79</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
+        <v>32</v>
+      </c>
+      <c r="B39" s="21">
+        <v>13</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="19">
         <v>33</v>
       </c>
-      <c r="B39" s="21">
+      <c r="B40" s="21">
         <v>14</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C40" s="19" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3436,7 +3445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merged changes from Previous Commit
</commit_message>
<xml_diff>
--- a/Project Plan and Resources/ProjectMonitor.xlsx
+++ b/Project Plan and Resources/ProjectMonitor.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="156">
   <si>
     <t>Resources</t>
   </si>
@@ -901,6 +901,12 @@
   <si>
     <t>can be solved by keeping track of a partition space usage - but this strategy seems complicated. - this is an NP hard 
 problem, the bin packing problem. http://stackoverflow.com/questions/16588669/spread-objects-evenly-over-multiple-collections</t>
+  </si>
+  <si>
+    <t>read from middle of a file.</t>
+  </si>
+  <si>
+    <t>how to keep track of the newly added edges?</t>
   </si>
 </sst>
 </file>
@@ -3292,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3699,6 +3705,20 @@
       </c>
       <c r="D32" s="17" t="s">
         <v>153</v>
+      </c>
+      <c r="E32" s="26">
+        <v>42250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="26">
+        <v>42253.811111111114</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Marked project plan issues.
</commit_message>
<xml_diff>
--- a/Project Plan and Resources/ProjectMonitor.xlsx
+++ b/Project Plan and Resources/ProjectMonitor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" tabRatio="869" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" tabRatio="869" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="4" r:id="rId1"/>
@@ -17,8 +17,7 @@
     <sheet name="Resources and GraphChi Info" sheetId="1" r:id="rId3"/>
     <sheet name="GraphChi Implementation Notes" sheetId="6" r:id="rId4"/>
     <sheet name="Issues" sheetId="3" r:id="rId5"/>
-    <sheet name="Research Qs and Motivation" sheetId="5" r:id="rId6"/>
-    <sheet name="Project Tool Usage" sheetId="7" r:id="rId7"/>
+    <sheet name="Project Tool Usage" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
   <si>
     <t>Resources</t>
   </si>
@@ -105,9 +104,6 @@
   </si>
   <si>
     <t>Concept Issue</t>
-  </si>
-  <si>
-    <t>Research Item</t>
   </si>
   <si>
     <t>Tasks</t>
@@ -283,9 +279,6 @@
   </si>
   <si>
     <t xml:space="preserve">Daily tasks may include high level goals and details. </t>
-  </si>
-  <si>
-    <t>These issues may include questions that arise during discussions, from reading other resources, or coding. These issues may or may not be mentioned elsewhere.</t>
   </si>
   <si>
     <t>* To get system Ready</t>
@@ -403,9 +396,6 @@
   </si>
   <si>
     <t>We'll need to calculate degree vertices.</t>
-  </si>
-  <si>
-    <t>Need to understand translation of vertices.</t>
   </si>
   <si>
     <r>
@@ -862,9 +852,6 @@
     <t>Cannot use arrayList for storing vertex degrees</t>
   </si>
   <si>
-    <t>This is because each element of an arraylist uses 8-12 bytes, that means 12 Gigs req for a graph of a billion vertices</t>
-  </si>
-  <si>
     <t>Each partition needs to have roughly the same number of edges.</t>
   </si>
   <si>
@@ -875,9 +862,6 @@
 than the partition size should be tackled</t>
   </si>
   <si>
-    <t>Just use max of the vertex of the max degree and the division (total number of edges/user given number of partitions)</t>
-  </si>
-  <si>
     <t>Corresponding to point 20, we also cannot just use an array, for we'll need to resize the array everytime we add a new element in the list, for which we shall need to copy the entire array, which may lead to outofmemory errors too.</t>
   </si>
   <si>
@@ -907,13 +891,75 @@
   </si>
   <si>
     <t>how to keep track of the newly added edges?</t>
+  </si>
+  <si>
+    <t>accounted</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>need to go through graphchi's plan</t>
+  </si>
+  <si>
+    <t>byte format</t>
+  </si>
+  <si>
+    <t>taken care of</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is because each element of an arraylist uses 8-12 bytes, that means 12 Gigs req for a graph of a billion vertices
+. Although this is less of a problem now as we shall not load the degrees of all the vertices, but only of those which are in
+the partitions loaded in the memory for computation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t>These issues may include questions that arise during discussions, from reading other resources, or coding. These issues may or may not be mentioned elsewhere.
+The striked out issues are dealt with,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> the ones in green are the ones that need to mentioned in the paper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">, the ones in yellow are the ones that don't need to be mentioned in the paper.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>We actually do use an array. Degree data structure only contains the counts which can be updated. In addition, we also
+need to initialize a new degrees file as per the sizes of the partitions being processed.</t>
+  </si>
+  <si>
+    <t>Can't, since there is a large number of vertices, we need int for degrees too.</t>
+  </si>
+  <si>
+    <t>This case has been handled.,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,8 +1019,15 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1020,6 +1073,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1193,6 +1252,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1204,6 +1278,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1488,7 +1583,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1507,18 +1602,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="37"/>
+      <c r="A1" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="3" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28"/>
@@ -1646,27 +1741,27 @@
     </row>
     <row r="5" spans="1:32" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
       <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="31" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
@@ -1872,7 +1967,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -2040,10 +2135,10 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2211,7 +2306,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2283,7 +2378,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -2306,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
@@ -2360,7 +2455,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2370,7 +2465,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2382,7 +2477,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2405,7 +2500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2420,17 +2515,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="A1" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -2460,7 +2555,7 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="16"/>
     </row>
@@ -2470,7 +2565,7 @@
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="16"/>
     </row>
@@ -2480,10 +2575,10 @@
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2492,7 +2587,7 @@
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="16"/>
     </row>
@@ -2502,7 +2597,7 @@
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="16"/>
     </row>
@@ -2512,7 +2607,7 @@
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="16"/>
     </row>
@@ -2522,7 +2617,7 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="16"/>
     </row>
@@ -2532,7 +2627,7 @@
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="16"/>
     </row>
@@ -2542,7 +2637,7 @@
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="16"/>
     </row>
@@ -2552,7 +2647,7 @@
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="16"/>
     </row>
@@ -2562,7 +2657,7 @@
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="16"/>
     </row>
@@ -2572,7 +2667,7 @@
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="16"/>
     </row>
@@ -2582,7 +2677,7 @@
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="16"/>
     </row>
@@ -2592,7 +2687,7 @@
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="16"/>
     </row>
@@ -2602,7 +2697,7 @@
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="16"/>
     </row>
@@ -2612,7 +2707,7 @@
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="16"/>
     </row>
@@ -2622,7 +2717,7 @@
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="16"/>
     </row>
@@ -2637,7 +2732,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2673,10 +2768,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2687,10 +2782,10 @@
         <v>6</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2701,7 +2796,7 @@
         <v>22</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>4</v>
@@ -2726,10 +2821,10 @@
         <v>10</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2737,13 +2832,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
@@ -2751,13 +2846,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2777,7 +2872,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2792,33 +2887,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+      <c r="A1" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>45</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2829,10 +2924,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2841,7 +2936,7 @@
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2853,7 +2948,7 @@
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -2865,14 +2960,14 @@
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
@@ -2880,10 +2975,10 @@
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2891,7 +2986,7 @@
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F9" s="25"/>
     </row>
@@ -2901,11 +2996,11 @@
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F10" s="23"/>
     </row>
@@ -2917,7 +3012,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2926,11 +3021,11 @@
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F12" s="23"/>
     </row>
@@ -2940,7 +3035,7 @@
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -2952,7 +3047,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="25"/>
@@ -2964,7 +3059,7 @@
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2976,7 +3071,7 @@
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -2988,7 +3083,7 @@
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -3000,11 +3095,11 @@
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" s="23"/>
     </row>
@@ -3014,7 +3109,7 @@
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="25"/>
@@ -3026,7 +3121,7 @@
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -3040,10 +3135,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -3054,10 +3149,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -3068,10 +3163,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -3080,7 +3175,7 @@
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -3092,7 +3187,7 @@
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -3104,7 +3199,7 @@
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -3116,7 +3211,7 @@
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -3128,7 +3223,7 @@
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
@@ -3142,7 +3237,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,10 +3248,10 @@
         <v>7</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3167,13 +3262,13 @@
         <v>8</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3184,18 +3279,18 @@
         <v>9</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E33" s="34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3206,7 +3301,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3217,17 +3312,17 @@
         <v>11</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B36" s="23"/>
       <c r="C36" s="23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F36" s="23"/>
     </row>
@@ -3236,7 +3331,7 @@
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
       <c r="E37" s="25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F37" s="23"/>
     </row>
@@ -3248,7 +3343,7 @@
         <v>12</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -3257,7 +3352,7 @@
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="23"/>
@@ -3271,7 +3366,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3282,7 +3377,7 @@
         <v>14</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3296,10 +3391,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3313,18 +3408,18 @@
     <col min="10" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
+    <row r="1" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -3343,398 +3438,464 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+    <row r="4" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="37">
         <v>42226.793749999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
+      <c r="D4" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="37"/>
+    </row>
+    <row r="5" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="37">
         <v>42226.793749999997</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="E5" s="37"/>
+    </row>
+    <row r="6" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="39">
         <v>42226.794444444444</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+      <c r="D6" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="39"/>
+    </row>
+    <row r="7" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35">
         <v>4</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="37">
         <v>42226.794444444444</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="E7" s="37"/>
+    </row>
+    <row r="8" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="35">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="26">
+      <c r="B8" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="37">
         <v>42227.967361111114</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+      <c r="D8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="37"/>
+    </row>
+    <row r="9" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="44">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="26">
+      <c r="B9" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="45">
         <v>42227.968055555553</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="D9" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="45"/>
+    </row>
+    <row r="10" spans="1:9" s="35" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="35">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="26">
+      <c r="B10" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="37">
         <v>42229.431944444441</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="37"/>
+    </row>
+    <row r="11" spans="1:9" s="38" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="39">
+        <v>42229.432638888888</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="39"/>
+    </row>
+    <row r="12" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>9</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>8</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="26">
-        <v>42229.432638888888</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>9</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="26">
+      <c r="C12" s="39">
         <v>42230.497916666667</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="D12" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="44">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="26">
+      <c r="B13" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="45">
         <v>42232.859722222223</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
+      <c r="D13" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="45"/>
+    </row>
+    <row r="14" spans="1:9" s="44" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="44">
         <v>11</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="26">
+      <c r="B14" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="45">
         <v>42232.90902777778</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="E14" s="45"/>
+    </row>
+    <row r="15" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="44">
         <v>12</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="26">
+      <c r="B15" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="45">
         <v>42232.92083333333</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="E15" s="45"/>
+    </row>
+    <row r="16" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="47">
         <v>13</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="48">
+        <v>42233.976388888892</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47">
+        <v>14</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="48">
+        <v>42234.688194444447</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47">
+        <v>15</v>
+      </c>
+      <c r="B18" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="26">
-        <v>42233.976388888892</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>14</v>
-      </c>
-      <c r="B17" s="14" t="s">
+      <c r="C18" s="48">
+        <v>42235.688194444447</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="47">
+        <v>16</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="48">
+        <v>42235.688194444447</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35">
+        <v>17</v>
+      </c>
+      <c r="B20" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="26">
-        <v>42234.688194444447</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
-        <v>15</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="26">
+      <c r="C20" s="37">
         <v>42235.688194444447</v>
       </c>
-      <c r="E18" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>16</v>
-      </c>
-      <c r="B19" s="14" t="s">
+      <c r="E20" s="37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="35">
+        <v>18</v>
+      </c>
+      <c r="B21" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="26">
-        <v>42235.688194444447</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>17</v>
-      </c>
-      <c r="B20" s="14" t="s">
+      <c r="C21" s="37">
+        <v>42236.643750000003</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="37"/>
+    </row>
+    <row r="22" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35">
+        <v>19</v>
+      </c>
+      <c r="B22" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="26">
-        <v>42235.688194444447</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>18</v>
-      </c>
-      <c r="B21" s="17" t="s">
+      <c r="C22" s="37">
+        <v>42236.644444444442</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="37"/>
+    </row>
+    <row r="23" spans="1:5" s="38" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="38">
+        <v>20</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="39">
+        <v>42242.896527777775</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35">
+        <v>21</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="26">
-        <v>42236.643750000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
+      <c r="C24" s="37">
+        <v>42242.898611111108</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="37"/>
+    </row>
+    <row r="25" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35">
+        <v>22</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="37">
+        <v>42242.898611111108</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="37"/>
+    </row>
+    <row r="26" spans="1:5" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="35">
+        <v>23</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="37">
+        <v>42242.9</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="37">
+        <v>42242.900694444441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="38" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="38">
+        <v>24</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="39">
+        <v>42242.907638888886</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="44">
+        <v>25</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="45">
+        <v>42242.972916666666</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28" s="45"/>
+    </row>
+    <row r="29" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="44">
+        <v>26</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="45">
+        <v>42249.696527777778</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="44">
+        <v>27</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="45">
+        <v>42249.697222222225</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="35" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="35">
+        <v>28</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="37">
+        <v>42250.004861111112</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="37"/>
+    </row>
+    <row r="32" spans="1:5" s="47" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="47">
+        <v>29</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="48">
+        <v>42250.089583333334</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="48">
+        <v>42250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="44">
+        <v>30</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" s="45">
+        <v>42253.811111111114</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" s="45"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="26">
-        <v>42236.644444444442</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>20</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C23" s="26">
-        <v>42242.896527777775</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>21</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="26">
-        <v>42242.898611111108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>22</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="26">
-        <v>42242.898611111108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>23</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C26" s="26">
-        <v>42242.9</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="26">
-        <v>42242.900694444441</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
-        <v>24</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="26">
-        <v>42242.907638888886</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
-        <v>25</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="26">
-        <v>42242.972916666666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
-        <v>26</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="26">
-        <v>42249.696527777778</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
-        <v>27</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="C30" s="26">
-        <v>42249.697222222225</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
-        <v>28</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="26">
-        <v>42250.004861111112</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
-        <v>29</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="26">
-        <v>42250.089583333334</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E32" s="26">
-        <v>42250</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" s="26">
-        <v>42253.811111111114</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="15" t="s">
+      <c r="D34" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E34" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3747,34 +3908,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -3790,12 +3923,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>